<commit_message>
integer values for service time
</commit_message>
<xml_diff>
--- a/Data_2024.xlsx
+++ b/Data_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongpeiguan/Documents/Teaching-2024-DMOR/2024_DMOR/CourseProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/tannerstaggs_ufl_edu/Documents/Code/dmor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F783A8C-B496-864B-B7DF-0D97232F377E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7F783A8C-B496-864B-B7DF-0D97232F377E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB9EEDDB-863F-41B3-9993-75DD099FB1D6}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="860" windowWidth="31820" windowHeight="19420" xr2:uid="{60757EBA-C529-5F4C-8302-EB839AC736F4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{60757EBA-C529-5F4C-8302-EB839AC736F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,11 +544,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86121C4-7FFA-6E4A-8664-A842C38542F2}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="5"/>
     <col min="3" max="3" width="14.33203125" style="5" customWidth="1"/>
@@ -561,7 +561,7 @@
     <col min="10" max="10" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -593,7 +593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -628,7 +628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -657,7 +657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -671,7 +671,7 @@
         <v>5500</v>
       </c>
       <c r="E4" s="4">
-        <v>34.722222222222221</v>
+        <v>34.7222222222222</v>
       </c>
       <c r="F4" s="2">
         <v>0.73263888888888884</v>
@@ -686,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -715,7 +715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -750,7 +750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -779,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -808,7 +808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -843,7 +843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -872,7 +872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -901,7 +901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -930,7 +930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -959,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -988,7 +988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1771,13 +1771,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D43" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D45" s="6"/>
     </row>
   </sheetData>

</xml_diff>